<commit_message>
removed the very large expanded file and added share of cumulative emissions
</commit_message>
<xml_diff>
--- a/stream3_visualization/Budget/Data/28-04-2025_ISO_Codes_Mapping.xlsx
+++ b/stream3_visualization/Budget/Data/28-04-2025_ISO_Codes_Mapping.xlsx
@@ -7,6 +7,11 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="caSIq22VOzKK6Ff0VJ8jG1yOWJwASQy1Fq0HNvVCbKk="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -160,7 +165,7 @@
     <t>AZE</t>
   </si>
   <si>
-    <t>Bahamas (the)</t>
+    <t xml:space="preserve">Bahamas </t>
   </si>
   <si>
     <t>BS</t>
@@ -250,7 +255,7 @@
     <t>BTN</t>
   </si>
   <si>
-    <t>Bolivia (Plurinational State of)</t>
+    <t>Bolivia</t>
   </si>
   <si>
     <t>BO</t>
@@ -304,7 +309,7 @@
     <t>BRA</t>
   </si>
   <si>
-    <t>British Indian Ocean Territory (the)</t>
+    <t>British Indian Ocean Territory</t>
   </si>
   <si>
     <t>IO</t>
@@ -385,7 +390,7 @@
     <t>CAN</t>
   </si>
   <si>
-    <t>Cayman Islands (the)</t>
+    <t>Cayman Islands</t>
   </si>
   <si>
     <t>KY</t>
@@ -394,7 +399,7 @@
     <t>CYM</t>
   </si>
   <si>
-    <t>Central African Republic (the)</t>
+    <t>Central African Republic</t>
   </si>
   <si>
     <t>CF</t>
@@ -439,7 +444,7 @@
     <t>CXR</t>
   </si>
   <si>
-    <t>Cocos (Keeling) Islands (the)</t>
+    <t>Cocos Islands</t>
   </si>
   <si>
     <t>CC</t>
@@ -457,7 +462,7 @@
     <t>COL</t>
   </si>
   <si>
-    <t>Comoros (the)</t>
+    <t>Comoros</t>
   </si>
   <si>
     <t>KM</t>
@@ -466,7 +471,7 @@
     <t>COM</t>
   </si>
   <si>
-    <t>Congo (the Democratic Republic of the)</t>
+    <t>Democratic Republic of the Congo</t>
   </si>
   <si>
     <t>CD</t>
@@ -475,7 +480,7 @@
     <t>COD</t>
   </si>
   <si>
-    <t>Congo (the)</t>
+    <t xml:space="preserve">Congo </t>
   </si>
   <si>
     <t>CG</t>
@@ -484,7 +489,7 @@
     <t>COG</t>
   </si>
   <si>
-    <t>Cook Islands (the)</t>
+    <t>Cook Islands</t>
   </si>
   <si>
     <t>CK</t>
@@ -583,7 +588,7 @@
     <t>DMA</t>
   </si>
   <si>
-    <t>Dominican Republic (the)</t>
+    <t xml:space="preserve">Dominican Republic </t>
   </si>
   <si>
     <t>DO</t>
@@ -664,7 +669,7 @@
     <t>ETH</t>
   </si>
   <si>
-    <t>Falkland Islands (the) [Malvinas]</t>
+    <t>Falkland Islands</t>
   </si>
   <si>
     <t>FK</t>
@@ -673,7 +678,7 @@
     <t>FLK</t>
   </si>
   <si>
-    <t>Faroe Islands (the)</t>
+    <t xml:space="preserve">Faroe Islands </t>
   </si>
   <si>
     <t>FO</t>
@@ -727,7 +732,7 @@
     <t>PYF</t>
   </si>
   <si>
-    <t>French Southern Territories (the)</t>
+    <t xml:space="preserve">French Southern Territories </t>
   </si>
   <si>
     <t>TF</t>
@@ -745,7 +750,7 @@
     <t>GAB</t>
   </si>
   <si>
-    <t>Gambia (the)</t>
+    <t xml:space="preserve">Gambia </t>
   </si>
   <si>
     <t>GM</t>
@@ -898,7 +903,7 @@
     <t>HMD</t>
   </si>
   <si>
-    <t>Holy See (the)</t>
+    <t>Holy See</t>
   </si>
   <si>
     <t>VA</t>
@@ -961,7 +966,7 @@
     <t>IDN</t>
   </si>
   <si>
-    <t>Iran (Islamic Republic of)</t>
+    <t>Iran</t>
   </si>
   <si>
     <t>IR</t>
@@ -1078,7 +1083,7 @@
     <t>KIR</t>
   </si>
   <si>
-    <t>Korea (the Democratic People's Republic of)</t>
+    <t>North Korea</t>
   </si>
   <si>
     <t>KP</t>
@@ -1087,7 +1092,7 @@
     <t>PRK</t>
   </si>
   <si>
-    <t>Korea (the Republic of)</t>
+    <t>South Korea</t>
   </si>
   <si>
     <t>KR</t>
@@ -1114,7 +1119,7 @@
     <t>KGZ</t>
   </si>
   <si>
-    <t>Lao People's Democratic Republic (the)</t>
+    <t>Lao People's Democratic Republic</t>
   </si>
   <si>
     <t>LA</t>
@@ -1258,7 +1263,7 @@
     <t>MLT</t>
   </si>
   <si>
-    <t>Marshall Islands (the)</t>
+    <t>Marshall Islands</t>
   </si>
   <si>
     <t>MH</t>
@@ -1312,7 +1317,7 @@
     <t>MEX</t>
   </si>
   <si>
-    <t>Micronesia (Federated States of)</t>
+    <t>Micronesia</t>
   </si>
   <si>
     <t>FM</t>
@@ -1321,7 +1326,7 @@
     <t>FSM</t>
   </si>
   <si>
-    <t>Moldova (the Republic of)</t>
+    <t xml:space="preserve">Moldova </t>
   </si>
   <si>
     <t>MD</t>
@@ -1420,7 +1425,7 @@
     <t>NPL</t>
   </si>
   <si>
-    <t>Netherlands (the)</t>
+    <t>Netherlands</t>
   </si>
   <si>
     <t>NL</t>
@@ -1456,7 +1461,7 @@
     <t>NIC</t>
   </si>
   <si>
-    <t>Niger (the)</t>
+    <t>Niger</t>
   </si>
   <si>
     <t>NE</t>
@@ -1492,7 +1497,7 @@
     <t>NFK</t>
   </si>
   <si>
-    <t>Northern Mariana Islands (the)</t>
+    <t>Northern Mariana Islands</t>
   </si>
   <si>
     <t>MP</t>
@@ -1582,7 +1587,7 @@
     <t>PER</t>
   </si>
   <si>
-    <t>Philippines (the)</t>
+    <t>Philippines</t>
   </si>
   <si>
     <t>PH</t>
@@ -1654,7 +1659,7 @@
     <t>ROU</t>
   </si>
   <si>
-    <t>Russian Federation (the)</t>
+    <t>Russia</t>
   </si>
   <si>
     <t>RU</t>
@@ -1915,7 +1920,7 @@
     <t>LKA</t>
   </si>
   <si>
-    <t>Sudan (the)</t>
+    <t>Sudan</t>
   </si>
   <si>
     <t>SD</t>
@@ -1969,7 +1974,7 @@
     <t>SYR</t>
   </si>
   <si>
-    <t>Taiwan (Province of China)</t>
+    <t>Taiwan</t>
   </si>
   <si>
     <t>TW</t>
@@ -1987,7 +1992,7 @@
     <t>TJK</t>
   </si>
   <si>
-    <t>Tanzania, United Republic of</t>
+    <t>Tanzania</t>
   </si>
   <si>
     <t>TZ</t>
@@ -2113,7 +2118,7 @@
     <t>UKR</t>
   </si>
   <si>
-    <t>United Arab Emirates (the)</t>
+    <t>United Arab Emirates</t>
   </si>
   <si>
     <t>AE</t>
@@ -2122,7 +2127,7 @@
     <t>ARE</t>
   </si>
   <si>
-    <t>United Kingdom of Great Britain and Northern Ireland (the)</t>
+    <t>United Kingdom</t>
   </si>
   <si>
     <t>GB</t>
@@ -2131,7 +2136,7 @@
     <t>GBR</t>
   </si>
   <si>
-    <t>United States Minor Outlying Islands (the)</t>
+    <t>United States Minor Outlying Islands</t>
   </si>
   <si>
     <t>UM</t>
@@ -2140,7 +2145,7 @@
     <t>UMI</t>
   </si>
   <si>
-    <t>United States of America (the)</t>
+    <t>United States of America</t>
   </si>
   <si>
     <t>US</t>
@@ -2176,7 +2181,7 @@
     <t>VUT</t>
   </si>
   <si>
-    <t>Venezuela (Bolivarian Republic of)</t>
+    <t>Venezuela</t>
   </si>
   <si>
     <t>VE</t>
@@ -2273,7 +2278,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2292,9 +2297,13 @@
       <name val="Inherit"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2345,19 +2354,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2572,13 +2582,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="52.75"/>
     <col customWidth="1" min="2" max="3" width="13.5"/>
+    <col customWidth="1" min="4" max="6" width="12.63"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2592,7 +2603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2606,7 +2617,7 @@
         <v>4.0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2620,7 +2631,7 @@
         <v>8.0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -2634,7 +2645,7 @@
         <v>12.0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -2648,7 +2659,7 @@
         <v>16.0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -2662,7 +2673,7 @@
         <v>20.0</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -2676,7 +2687,7 @@
         <v>24.0</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -2690,7 +2701,7 @@
         <v>660.0</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2704,7 +2715,7 @@
         <v>10.0</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
@@ -2718,7 +2729,7 @@
         <v>28.0</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
@@ -2732,7 +2743,7 @@
         <v>32.0</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -2746,7 +2757,7 @@
         <v>51.0</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
@@ -2760,7 +2771,7 @@
         <v>533.0</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -2774,7 +2785,7 @@
         <v>36.0</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
@@ -2788,8 +2799,8 @@
         <v>40.0</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2802,8 +2813,8 @@
         <v>31.0</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="2" t="s">
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2816,7 +2827,7 @@
         <v>44.0</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>52</v>
       </c>
@@ -2830,7 +2841,7 @@
         <v>48.0</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>55</v>
       </c>
@@ -2844,7 +2855,7 @@
         <v>50.0</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>58</v>
       </c>
@@ -2858,7 +2869,7 @@
         <v>52.0</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>61</v>
       </c>
@@ -2872,7 +2883,7 @@
         <v>112.0</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>64</v>
       </c>
@@ -2886,7 +2897,7 @@
         <v>56.0</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>67</v>
       </c>
@@ -2900,7 +2911,7 @@
         <v>84.0</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>70</v>
       </c>
@@ -2914,7 +2925,7 @@
         <v>204.0</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>73</v>
       </c>
@@ -2928,7 +2939,7 @@
         <v>60.0</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
@@ -2942,8 +2953,8 @@
         <v>64.0</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="2" t="s">
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2956,7 +2967,7 @@
         <v>68.0</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>82</v>
       </c>
@@ -2970,7 +2981,7 @@
         <v>535.0</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>85</v>
       </c>
@@ -2984,7 +2995,7 @@
         <v>70.0</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>88</v>
       </c>
@@ -2998,7 +3009,7 @@
         <v>72.0</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>91</v>
       </c>
@@ -3012,7 +3023,7 @@
         <v>74.0</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>94</v>
       </c>
@@ -3026,8 +3037,8 @@
         <v>76.0</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="2" t="s">
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -3040,7 +3051,7 @@
         <v>86.0</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>100</v>
       </c>
@@ -3054,7 +3065,7 @@
         <v>96.0</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>103</v>
       </c>
@@ -3068,7 +3079,7 @@
         <v>100.0</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>106</v>
       </c>
@@ -3082,7 +3093,7 @@
         <v>854.0</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
@@ -3096,7 +3107,7 @@
         <v>108.0</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
@@ -3110,7 +3121,7 @@
         <v>132.0</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
@@ -3124,7 +3135,7 @@
         <v>116.0</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>118</v>
       </c>
@@ -3138,7 +3149,7 @@
         <v>120.0</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>121</v>
       </c>
@@ -3152,8 +3163,8 @@
         <v>124.0</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="2" t="s">
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -3166,8 +3177,8 @@
         <v>136.0</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="2" t="s">
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -3180,7 +3191,7 @@
         <v>140.0</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>130</v>
       </c>
@@ -3194,7 +3205,7 @@
         <v>148.0</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>133</v>
       </c>
@@ -3208,7 +3219,7 @@
         <v>152.0</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>136</v>
       </c>
@@ -3222,7 +3233,7 @@
         <v>156.0</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>139</v>
       </c>
@@ -3236,8 +3247,8 @@
         <v>162.0</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="2" t="s">
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="3" t="s">
         <v>142</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -3250,7 +3261,7 @@
         <v>166.0</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>145</v>
       </c>
@@ -3264,8 +3275,8 @@
         <v>170.0</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="2" t="s">
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -3278,8 +3289,8 @@
         <v>174.0</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="2" t="s">
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="3" t="s">
         <v>151</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -3292,8 +3303,8 @@
         <v>180.0</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="2" t="s">
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="3" t="s">
         <v>154</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -3306,8 +3317,8 @@
         <v>178.0</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="2" t="s">
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -3320,7 +3331,7 @@
         <v>184.0</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="2" t="s">
         <v>160</v>
       </c>
@@ -3334,7 +3345,7 @@
         <v>188.0</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>163</v>
       </c>
@@ -3348,7 +3359,7 @@
         <v>191.0</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>166</v>
       </c>
@@ -3362,7 +3373,7 @@
         <v>192.0</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>169</v>
       </c>
@@ -3376,7 +3387,7 @@
         <v>531.0</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>172</v>
       </c>
@@ -3390,7 +3401,7 @@
         <v>196.0</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="2" t="s">
         <v>175</v>
       </c>
@@ -3404,7 +3415,7 @@
         <v>203.0</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="2" t="s">
         <v>178</v>
       </c>
@@ -3418,7 +3429,7 @@
         <v>384.0</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="2" t="s">
         <v>181</v>
       </c>
@@ -3432,7 +3443,7 @@
         <v>208.0</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="2" t="s">
         <v>184</v>
       </c>
@@ -3446,7 +3457,7 @@
         <v>262.0</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="2" t="s">
         <v>187</v>
       </c>
@@ -3460,8 +3471,8 @@
         <v>212.0</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="2" t="s">
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="A64" s="3" t="s">
         <v>190</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -3474,7 +3485,7 @@
         <v>214.0</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="2" t="s">
         <v>193</v>
       </c>
@@ -3488,7 +3499,7 @@
         <v>218.0</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="2" t="s">
         <v>196</v>
       </c>
@@ -3502,7 +3513,7 @@
         <v>818.0</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="2" t="s">
         <v>199</v>
       </c>
@@ -3516,7 +3527,7 @@
         <v>222.0</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="2" t="s">
         <v>202</v>
       </c>
@@ -3530,7 +3541,7 @@
         <v>226.0</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="2" t="s">
         <v>205</v>
       </c>
@@ -3544,7 +3555,7 @@
         <v>232.0</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="2" t="s">
         <v>208</v>
       </c>
@@ -3558,7 +3569,7 @@
         <v>233.0</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="2" t="s">
         <v>211</v>
       </c>
@@ -3572,8 +3583,8 @@
         <v>748.0</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="2" t="s">
+    <row r="72" ht="15.75" customHeight="1">
+      <c r="A72" s="3" t="s">
         <v>214</v>
       </c>
       <c r="B72" s="2" t="s">
@@ -3586,8 +3597,8 @@
         <v>231.0</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" s="2" t="s">
+    <row r="73" ht="15.75" customHeight="1">
+      <c r="A73" s="3" t="s">
         <v>217</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -3600,8 +3611,8 @@
         <v>238.0</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="2" t="s">
+    <row r="74" ht="15.75" customHeight="1">
+      <c r="A74" s="3" t="s">
         <v>220</v>
       </c>
       <c r="B74" s="2" t="s">
@@ -3614,7 +3625,7 @@
         <v>234.0</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="2" t="s">
         <v>223</v>
       </c>
@@ -3628,7 +3639,7 @@
         <v>242.0</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="2" t="s">
         <v>226</v>
       </c>
@@ -3642,7 +3653,7 @@
         <v>246.0</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="2" t="s">
         <v>229</v>
       </c>
@@ -3656,7 +3667,7 @@
         <v>250.0</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="2" t="s">
         <v>232</v>
       </c>
@@ -3670,7 +3681,7 @@
         <v>254.0</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="2" t="s">
         <v>235</v>
       </c>
@@ -3684,8 +3695,8 @@
         <v>258.0</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="2" t="s">
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="A80" s="3" t="s">
         <v>238</v>
       </c>
       <c r="B80" s="2" t="s">
@@ -3698,7 +3709,7 @@
         <v>260.0</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="2" t="s">
         <v>241</v>
       </c>
@@ -3712,8 +3723,8 @@
         <v>266.0</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" s="2" t="s">
+    <row r="82" ht="15.75" customHeight="1">
+      <c r="A82" s="3" t="s">
         <v>244</v>
       </c>
       <c r="B82" s="2" t="s">
@@ -3726,7 +3737,7 @@
         <v>270.0</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="2" t="s">
         <v>247</v>
       </c>
@@ -3740,7 +3751,7 @@
         <v>268.0</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="2" t="s">
         <v>250</v>
       </c>
@@ -3754,7 +3765,7 @@
         <v>276.0</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="2" t="s">
         <v>253</v>
       </c>
@@ -3768,7 +3779,7 @@
         <v>288.0</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="2" t="s">
         <v>256</v>
       </c>
@@ -3782,7 +3793,7 @@
         <v>292.0</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="2" t="s">
         <v>259</v>
       </c>
@@ -3796,7 +3807,7 @@
         <v>300.0</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="2" t="s">
         <v>262</v>
       </c>
@@ -3810,7 +3821,7 @@
         <v>304.0</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="2" t="s">
         <v>265</v>
       </c>
@@ -3824,7 +3835,7 @@
         <v>308.0</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="2" t="s">
         <v>268</v>
       </c>
@@ -3838,7 +3849,7 @@
         <v>312.0</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="2" t="s">
         <v>271</v>
       </c>
@@ -3852,7 +3863,7 @@
         <v>316.0</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="2" t="s">
         <v>274</v>
       </c>
@@ -3866,7 +3877,7 @@
         <v>320.0</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="2" t="s">
         <v>277</v>
       </c>
@@ -3880,7 +3891,7 @@
         <v>831.0</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="2" t="s">
         <v>280</v>
       </c>
@@ -3894,7 +3905,7 @@
         <v>324.0</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="2" t="s">
         <v>283</v>
       </c>
@@ -3908,7 +3919,7 @@
         <v>624.0</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="2" t="s">
         <v>286</v>
       </c>
@@ -3922,7 +3933,7 @@
         <v>328.0</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="2" t="s">
         <v>289</v>
       </c>
@@ -3936,7 +3947,7 @@
         <v>332.0</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="2" t="s">
         <v>292</v>
       </c>
@@ -3950,8 +3961,8 @@
         <v>334.0</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" s="2" t="s">
+    <row r="99" ht="15.75" customHeight="1">
+      <c r="A99" s="3" t="s">
         <v>295</v>
       </c>
       <c r="B99" s="2" t="s">
@@ -3964,7 +3975,7 @@
         <v>336.0</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="2" t="s">
         <v>298</v>
       </c>
@@ -3978,7 +3989,7 @@
         <v>340.0</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="2" t="s">
         <v>301</v>
       </c>
@@ -3992,7 +4003,7 @@
         <v>344.0</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="2" t="s">
         <v>304</v>
       </c>
@@ -4006,7 +4017,7 @@
         <v>348.0</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="2" t="s">
         <v>307</v>
       </c>
@@ -4020,7 +4031,7 @@
         <v>352.0</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="2" t="s">
         <v>310</v>
       </c>
@@ -4034,7 +4045,7 @@
         <v>356.0</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="2" t="s">
         <v>313</v>
       </c>
@@ -4048,8 +4059,8 @@
         <v>360.0</v>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" s="2" t="s">
+    <row r="106" ht="15.75" customHeight="1">
+      <c r="A106" s="3" t="s">
         <v>316</v>
       </c>
       <c r="B106" s="2" t="s">
@@ -4062,7 +4073,7 @@
         <v>364.0</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="2" t="s">
         <v>319</v>
       </c>
@@ -4076,7 +4087,7 @@
         <v>368.0</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="2" t="s">
         <v>322</v>
       </c>
@@ -4090,7 +4101,7 @@
         <v>372.0</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="2" t="s">
         <v>325</v>
       </c>
@@ -4104,7 +4115,7 @@
         <v>833.0</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="2" t="s">
         <v>328</v>
       </c>
@@ -4118,7 +4129,7 @@
         <v>376.0</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="2" t="s">
         <v>331</v>
       </c>
@@ -4132,7 +4143,7 @@
         <v>380.0</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="2" t="s">
         <v>334</v>
       </c>
@@ -4146,7 +4157,7 @@
         <v>388.0</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="2" t="s">
         <v>337</v>
       </c>
@@ -4160,7 +4171,7 @@
         <v>392.0</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="2" t="s">
         <v>340</v>
       </c>
@@ -4174,7 +4185,7 @@
         <v>832.0</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="2" t="s">
         <v>343</v>
       </c>
@@ -4188,7 +4199,7 @@
         <v>400.0</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="2" t="s">
         <v>346</v>
       </c>
@@ -4202,7 +4213,7 @@
         <v>398.0</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="2" t="s">
         <v>349</v>
       </c>
@@ -4216,7 +4227,7 @@
         <v>404.0</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="2" t="s">
         <v>352</v>
       </c>
@@ -4230,8 +4241,8 @@
         <v>296.0</v>
       </c>
     </row>
-    <row r="119">
-      <c r="A119" s="2" t="s">
+    <row r="119" ht="15.75" customHeight="1">
+      <c r="A119" s="3" t="s">
         <v>355</v>
       </c>
       <c r="B119" s="2" t="s">
@@ -4244,8 +4255,8 @@
         <v>408.0</v>
       </c>
     </row>
-    <row r="120">
-      <c r="A120" s="2" t="s">
+    <row r="120" ht="15.75" customHeight="1">
+      <c r="A120" s="3" t="s">
         <v>358</v>
       </c>
       <c r="B120" s="2" t="s">
@@ -4258,7 +4269,7 @@
         <v>410.0</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="2" t="s">
         <v>361</v>
       </c>
@@ -4272,7 +4283,7 @@
         <v>414.0</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="2" t="s">
         <v>364</v>
       </c>
@@ -4286,8 +4297,8 @@
         <v>417.0</v>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" s="2" t="s">
+    <row r="123" ht="15.75" customHeight="1">
+      <c r="A123" s="3" t="s">
         <v>367</v>
       </c>
       <c r="B123" s="2" t="s">
@@ -4300,7 +4311,7 @@
         <v>418.0</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="2" t="s">
         <v>370</v>
       </c>
@@ -4314,7 +4325,7 @@
         <v>428.0</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="2" t="s">
         <v>373</v>
       </c>
@@ -4328,7 +4339,7 @@
         <v>422.0</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="2" t="s">
         <v>376</v>
       </c>
@@ -4342,7 +4353,7 @@
         <v>426.0</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="2" t="s">
         <v>379</v>
       </c>
@@ -4356,7 +4367,7 @@
         <v>430.0</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="2" t="s">
         <v>382</v>
       </c>
@@ -4370,7 +4381,7 @@
         <v>434.0</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="2" t="s">
         <v>385</v>
       </c>
@@ -4384,7 +4395,7 @@
         <v>438.0</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="2" t="s">
         <v>388</v>
       </c>
@@ -4398,7 +4409,7 @@
         <v>440.0</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="2" t="s">
         <v>391</v>
       </c>
@@ -4412,7 +4423,7 @@
         <v>442.0</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="2" t="s">
         <v>394</v>
       </c>
@@ -4426,7 +4437,7 @@
         <v>446.0</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="2" t="s">
         <v>397</v>
       </c>
@@ -4440,7 +4451,7 @@
         <v>450.0</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="2" t="s">
         <v>400</v>
       </c>
@@ -4454,7 +4465,7 @@
         <v>454.0</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="2" t="s">
         <v>403</v>
       </c>
@@ -4468,7 +4479,7 @@
         <v>458.0</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="2" t="s">
         <v>406</v>
       </c>
@@ -4482,7 +4493,7 @@
         <v>462.0</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" ht="15.75" customHeight="1">
       <c r="A137" s="2" t="s">
         <v>409</v>
       </c>
@@ -4496,7 +4507,7 @@
         <v>466.0</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="2" t="s">
         <v>412</v>
       </c>
@@ -4510,8 +4521,8 @@
         <v>470.0</v>
       </c>
     </row>
-    <row r="139">
-      <c r="A139" s="2" t="s">
+    <row r="139" ht="15.75" customHeight="1">
+      <c r="A139" s="3" t="s">
         <v>415</v>
       </c>
       <c r="B139" s="2" t="s">
@@ -4524,7 +4535,7 @@
         <v>584.0</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="2" t="s">
         <v>418</v>
       </c>
@@ -4538,7 +4549,7 @@
         <v>474.0</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="2" t="s">
         <v>421</v>
       </c>
@@ -4552,7 +4563,7 @@
         <v>478.0</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="2" t="s">
         <v>424</v>
       </c>
@@ -4566,7 +4577,7 @@
         <v>480.0</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" ht="15.75" customHeight="1">
       <c r="A143" s="2" t="s">
         <v>427</v>
       </c>
@@ -4580,7 +4591,7 @@
         <v>175.0</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="2" t="s">
         <v>430</v>
       </c>
@@ -4594,8 +4605,8 @@
         <v>484.0</v>
       </c>
     </row>
-    <row r="145">
-      <c r="A145" s="2" t="s">
+    <row r="145" ht="15.75" customHeight="1">
+      <c r="A145" s="3" t="s">
         <v>433</v>
       </c>
       <c r="B145" s="2" t="s">
@@ -4608,8 +4619,8 @@
         <v>583.0</v>
       </c>
     </row>
-    <row r="146">
-      <c r="A146" s="2" t="s">
+    <row r="146" ht="15.75" customHeight="1">
+      <c r="A146" s="3" t="s">
         <v>436</v>
       </c>
       <c r="B146" s="2" t="s">
@@ -4622,7 +4633,7 @@
         <v>498.0</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" ht="15.75" customHeight="1">
       <c r="A147" s="2" t="s">
         <v>439</v>
       </c>
@@ -4636,7 +4647,7 @@
         <v>492.0</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="2" t="s">
         <v>442</v>
       </c>
@@ -4650,7 +4661,7 @@
         <v>496.0</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="2" t="s">
         <v>445</v>
       </c>
@@ -4664,7 +4675,7 @@
         <v>499.0</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="2" t="s">
         <v>448</v>
       </c>
@@ -4678,7 +4689,7 @@
         <v>500.0</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="2" t="s">
         <v>451</v>
       </c>
@@ -4692,7 +4703,7 @@
         <v>504.0</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="2" t="s">
         <v>454</v>
       </c>
@@ -4706,7 +4717,7 @@
         <v>508.0</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="2" t="s">
         <v>457</v>
       </c>
@@ -4720,7 +4731,7 @@
         <v>104.0</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" ht="15.75" customHeight="1">
       <c r="A154" s="2" t="s">
         <v>460</v>
       </c>
@@ -4734,7 +4745,7 @@
         <v>516.0</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="2" t="s">
         <v>463</v>
       </c>
@@ -4748,7 +4759,7 @@
         <v>520.0</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="2" t="s">
         <v>466</v>
       </c>
@@ -4762,8 +4773,8 @@
         <v>524.0</v>
       </c>
     </row>
-    <row r="157">
-      <c r="A157" s="2" t="s">
+    <row r="157" ht="15.75" customHeight="1">
+      <c r="A157" s="3" t="s">
         <v>469</v>
       </c>
       <c r="B157" s="2" t="s">
@@ -4776,7 +4787,7 @@
         <v>528.0</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="2" t="s">
         <v>472</v>
       </c>
@@ -4790,7 +4801,7 @@
         <v>540.0</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="2" t="s">
         <v>475</v>
       </c>
@@ -4804,7 +4815,7 @@
         <v>554.0</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="2" t="s">
         <v>478</v>
       </c>
@@ -4818,8 +4829,8 @@
         <v>558.0</v>
       </c>
     </row>
-    <row r="161">
-      <c r="A161" s="2" t="s">
+    <row r="161" ht="15.75" customHeight="1">
+      <c r="A161" s="3" t="s">
         <v>481</v>
       </c>
       <c r="B161" s="2" t="s">
@@ -4832,7 +4843,7 @@
         <v>562.0</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="2" t="s">
         <v>484</v>
       </c>
@@ -4846,7 +4857,7 @@
         <v>566.0</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="2" t="s">
         <v>487</v>
       </c>
@@ -4860,7 +4871,7 @@
         <v>570.0</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="2" t="s">
         <v>490</v>
       </c>
@@ -4874,8 +4885,8 @@
         <v>574.0</v>
       </c>
     </row>
-    <row r="165">
-      <c r="A165" s="2" t="s">
+    <row r="165" ht="15.75" customHeight="1">
+      <c r="A165" s="3" t="s">
         <v>493</v>
       </c>
       <c r="B165" s="2" t="s">
@@ -4888,7 +4899,7 @@
         <v>580.0</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" ht="15.75" customHeight="1">
       <c r="A166" s="2" t="s">
         <v>496</v>
       </c>
@@ -4902,7 +4913,7 @@
         <v>578.0</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" ht="15.75" customHeight="1">
       <c r="A167" s="2" t="s">
         <v>499</v>
       </c>
@@ -4916,7 +4927,7 @@
         <v>512.0</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" ht="15.75" customHeight="1">
       <c r="A168" s="2" t="s">
         <v>502</v>
       </c>
@@ -4930,7 +4941,7 @@
         <v>586.0</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="2" t="s">
         <v>505</v>
       </c>
@@ -4944,7 +4955,7 @@
         <v>585.0</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" ht="15.75" customHeight="1">
       <c r="A170" s="2" t="s">
         <v>508</v>
       </c>
@@ -4958,7 +4969,7 @@
         <v>275.0</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" ht="15.75" customHeight="1">
       <c r="A171" s="2" t="s">
         <v>511</v>
       </c>
@@ -4972,7 +4983,7 @@
         <v>591.0</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" ht="15.75" customHeight="1">
       <c r="A172" s="2" t="s">
         <v>514</v>
       </c>
@@ -4986,7 +4997,7 @@
         <v>598.0</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" ht="15.75" customHeight="1">
       <c r="A173" s="2" t="s">
         <v>517</v>
       </c>
@@ -5000,7 +5011,7 @@
         <v>600.0</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" ht="15.75" customHeight="1">
       <c r="A174" s="2" t="s">
         <v>520</v>
       </c>
@@ -5014,8 +5025,8 @@
         <v>604.0</v>
       </c>
     </row>
-    <row r="175">
-      <c r="A175" s="2" t="s">
+    <row r="175" ht="15.75" customHeight="1">
+      <c r="A175" s="3" t="s">
         <v>523</v>
       </c>
       <c r="B175" s="2" t="s">
@@ -5028,7 +5039,7 @@
         <v>608.0</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" ht="15.75" customHeight="1">
       <c r="A176" s="2" t="s">
         <v>526</v>
       </c>
@@ -5042,7 +5053,7 @@
         <v>612.0</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" ht="15.75" customHeight="1">
       <c r="A177" s="2" t="s">
         <v>529</v>
       </c>
@@ -5056,7 +5067,7 @@
         <v>616.0</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" ht="15.75" customHeight="1">
       <c r="A178" s="2" t="s">
         <v>532</v>
       </c>
@@ -5070,7 +5081,7 @@
         <v>620.0</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" ht="15.75" customHeight="1">
       <c r="A179" s="2" t="s">
         <v>535</v>
       </c>
@@ -5084,7 +5095,7 @@
         <v>630.0</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" ht="15.75" customHeight="1">
       <c r="A180" s="2" t="s">
         <v>538</v>
       </c>
@@ -5098,7 +5109,7 @@
         <v>634.0</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" ht="15.75" customHeight="1">
       <c r="A181" s="2" t="s">
         <v>541</v>
       </c>
@@ -5112,7 +5123,7 @@
         <v>807.0</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" ht="15.75" customHeight="1">
       <c r="A182" s="2" t="s">
         <v>544</v>
       </c>
@@ -5126,8 +5137,8 @@
         <v>642.0</v>
       </c>
     </row>
-    <row r="183">
-      <c r="A183" s="2" t="s">
+    <row r="183" ht="15.75" customHeight="1">
+      <c r="A183" s="3" t="s">
         <v>547</v>
       </c>
       <c r="B183" s="2" t="s">
@@ -5140,7 +5151,7 @@
         <v>643.0</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" ht="15.75" customHeight="1">
       <c r="A184" s="2" t="s">
         <v>550</v>
       </c>
@@ -5154,7 +5165,7 @@
         <v>646.0</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" ht="15.75" customHeight="1">
       <c r="A185" s="2" t="s">
         <v>553</v>
       </c>
@@ -5168,7 +5179,7 @@
         <v>638.0</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" ht="15.75" customHeight="1">
       <c r="A186" s="2" t="s">
         <v>556</v>
       </c>
@@ -5182,7 +5193,7 @@
         <v>652.0</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" ht="15.75" customHeight="1">
       <c r="A187" s="2" t="s">
         <v>559</v>
       </c>
@@ -5196,7 +5207,7 @@
         <v>654.0</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" ht="15.75" customHeight="1">
       <c r="A188" s="2" t="s">
         <v>562</v>
       </c>
@@ -5210,7 +5221,7 @@
         <v>659.0</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" ht="15.75" customHeight="1">
       <c r="A189" s="2" t="s">
         <v>565</v>
       </c>
@@ -5224,7 +5235,7 @@
         <v>662.0</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" ht="15.75" customHeight="1">
       <c r="A190" s="2" t="s">
         <v>568</v>
       </c>
@@ -5238,7 +5249,7 @@
         <v>663.0</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" ht="15.75" customHeight="1">
       <c r="A191" s="2" t="s">
         <v>571</v>
       </c>
@@ -5252,7 +5263,7 @@
         <v>666.0</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" ht="15.75" customHeight="1">
       <c r="A192" s="2" t="s">
         <v>574</v>
       </c>
@@ -5266,7 +5277,7 @@
         <v>670.0</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" ht="15.75" customHeight="1">
       <c r="A193" s="2" t="s">
         <v>577</v>
       </c>
@@ -5280,7 +5291,7 @@
         <v>882.0</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" ht="15.75" customHeight="1">
       <c r="A194" s="2" t="s">
         <v>580</v>
       </c>
@@ -5294,7 +5305,7 @@
         <v>674.0</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" ht="15.75" customHeight="1">
       <c r="A195" s="2" t="s">
         <v>583</v>
       </c>
@@ -5308,7 +5319,7 @@
         <v>678.0</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" ht="15.75" customHeight="1">
       <c r="A196" s="2" t="s">
         <v>586</v>
       </c>
@@ -5322,7 +5333,7 @@
         <v>682.0</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" ht="15.75" customHeight="1">
       <c r="A197" s="2" t="s">
         <v>589</v>
       </c>
@@ -5336,7 +5347,7 @@
         <v>686.0</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" ht="15.75" customHeight="1">
       <c r="A198" s="2" t="s">
         <v>592</v>
       </c>
@@ -5350,7 +5361,7 @@
         <v>688.0</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" ht="15.75" customHeight="1">
       <c r="A199" s="2" t="s">
         <v>595</v>
       </c>
@@ -5364,7 +5375,7 @@
         <v>690.0</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" ht="15.75" customHeight="1">
       <c r="A200" s="2" t="s">
         <v>598</v>
       </c>
@@ -5378,7 +5389,7 @@
         <v>694.0</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" ht="15.75" customHeight="1">
       <c r="A201" s="2" t="s">
         <v>601</v>
       </c>
@@ -5392,7 +5403,7 @@
         <v>702.0</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" ht="15.75" customHeight="1">
       <c r="A202" s="2" t="s">
         <v>604</v>
       </c>
@@ -5406,7 +5417,7 @@
         <v>534.0</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" ht="15.75" customHeight="1">
       <c r="A203" s="2" t="s">
         <v>607</v>
       </c>
@@ -5420,7 +5431,7 @@
         <v>703.0</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" ht="15.75" customHeight="1">
       <c r="A204" s="2" t="s">
         <v>610</v>
       </c>
@@ -5434,7 +5445,7 @@
         <v>705.0</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" ht="15.75" customHeight="1">
       <c r="A205" s="2" t="s">
         <v>613</v>
       </c>
@@ -5448,7 +5459,7 @@
         <v>90.0</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" ht="15.75" customHeight="1">
       <c r="A206" s="2" t="s">
         <v>616</v>
       </c>
@@ -5462,7 +5473,7 @@
         <v>706.0</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" ht="15.75" customHeight="1">
       <c r="A207" s="2" t="s">
         <v>619</v>
       </c>
@@ -5476,7 +5487,7 @@
         <v>710.0</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" ht="15.75" customHeight="1">
       <c r="A208" s="2" t="s">
         <v>622</v>
       </c>
@@ -5490,7 +5501,7 @@
         <v>239.0</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" ht="15.75" customHeight="1">
       <c r="A209" s="2" t="s">
         <v>625</v>
       </c>
@@ -5504,7 +5515,7 @@
         <v>728.0</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" ht="15.75" customHeight="1">
       <c r="A210" s="2" t="s">
         <v>628</v>
       </c>
@@ -5518,7 +5529,7 @@
         <v>724.0</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" ht="15.75" customHeight="1">
       <c r="A211" s="2" t="s">
         <v>631</v>
       </c>
@@ -5532,8 +5543,8 @@
         <v>144.0</v>
       </c>
     </row>
-    <row r="212">
-      <c r="A212" s="2" t="s">
+    <row r="212" ht="15.75" customHeight="1">
+      <c r="A212" s="3" t="s">
         <v>634</v>
       </c>
       <c r="B212" s="2" t="s">
@@ -5546,7 +5557,7 @@
         <v>729.0</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" ht="15.75" customHeight="1">
       <c r="A213" s="2" t="s">
         <v>637</v>
       </c>
@@ -5560,7 +5571,7 @@
         <v>740.0</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" ht="15.75" customHeight="1">
       <c r="A214" s="2" t="s">
         <v>640</v>
       </c>
@@ -5574,7 +5585,7 @@
         <v>744.0</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" ht="15.75" customHeight="1">
       <c r="A215" s="2" t="s">
         <v>643</v>
       </c>
@@ -5588,7 +5599,7 @@
         <v>752.0</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" ht="15.75" customHeight="1">
       <c r="A216" s="2" t="s">
         <v>646</v>
       </c>
@@ -5602,7 +5613,7 @@
         <v>756.0</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" ht="15.75" customHeight="1">
       <c r="A217" s="2" t="s">
         <v>649</v>
       </c>
@@ -5616,8 +5627,8 @@
         <v>760.0</v>
       </c>
     </row>
-    <row r="218">
-      <c r="A218" s="2" t="s">
+    <row r="218" ht="15.75" customHeight="1">
+      <c r="A218" s="3" t="s">
         <v>652</v>
       </c>
       <c r="B218" s="2" t="s">
@@ -5630,7 +5641,7 @@
         <v>158.0</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" ht="15.75" customHeight="1">
       <c r="A219" s="2" t="s">
         <v>655</v>
       </c>
@@ -5644,8 +5655,8 @@
         <v>762.0</v>
       </c>
     </row>
-    <row r="220">
-      <c r="A220" s="2" t="s">
+    <row r="220" ht="15.75" customHeight="1">
+      <c r="A220" s="3" t="s">
         <v>658</v>
       </c>
       <c r="B220" s="2" t="s">
@@ -5658,7 +5669,7 @@
         <v>834.0</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" ht="15.75" customHeight="1">
       <c r="A221" s="2" t="s">
         <v>661</v>
       </c>
@@ -5672,7 +5683,7 @@
         <v>764.0</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" ht="15.75" customHeight="1">
       <c r="A222" s="2" t="s">
         <v>664</v>
       </c>
@@ -5686,7 +5697,7 @@
         <v>626.0</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" ht="15.75" customHeight="1">
       <c r="A223" s="2" t="s">
         <v>667</v>
       </c>
@@ -5700,7 +5711,7 @@
         <v>768.0</v>
       </c>
     </row>
-    <row r="224">
+    <row r="224" ht="15.75" customHeight="1">
       <c r="A224" s="2" t="s">
         <v>670</v>
       </c>
@@ -5714,7 +5725,7 @@
         <v>772.0</v>
       </c>
     </row>
-    <row r="225">
+    <row r="225" ht="15.75" customHeight="1">
       <c r="A225" s="2" t="s">
         <v>673</v>
       </c>
@@ -5728,7 +5739,7 @@
         <v>776.0</v>
       </c>
     </row>
-    <row r="226">
+    <row r="226" ht="15.75" customHeight="1">
       <c r="A226" s="2" t="s">
         <v>676</v>
       </c>
@@ -5742,7 +5753,7 @@
         <v>780.0</v>
       </c>
     </row>
-    <row r="227">
+    <row r="227" ht="15.75" customHeight="1">
       <c r="A227" s="2" t="s">
         <v>679</v>
       </c>
@@ -5756,7 +5767,7 @@
         <v>788.0</v>
       </c>
     </row>
-    <row r="228">
+    <row r="228" ht="15.75" customHeight="1">
       <c r="A228" s="2" t="s">
         <v>682</v>
       </c>
@@ -5770,7 +5781,7 @@
         <v>792.0</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" ht="15.75" customHeight="1">
       <c r="A229" s="2" t="s">
         <v>685</v>
       </c>
@@ -5784,7 +5795,7 @@
         <v>795.0</v>
       </c>
     </row>
-    <row r="230">
+    <row r="230" ht="15.75" customHeight="1">
       <c r="A230" s="2" t="s">
         <v>688</v>
       </c>
@@ -5798,7 +5809,7 @@
         <v>796.0</v>
       </c>
     </row>
-    <row r="231">
+    <row r="231" ht="15.75" customHeight="1">
       <c r="A231" s="2" t="s">
         <v>691</v>
       </c>
@@ -5812,7 +5823,7 @@
         <v>798.0</v>
       </c>
     </row>
-    <row r="232">
+    <row r="232" ht="15.75" customHeight="1">
       <c r="A232" s="2" t="s">
         <v>694</v>
       </c>
@@ -5826,7 +5837,7 @@
         <v>800.0</v>
       </c>
     </row>
-    <row r="233">
+    <row r="233" ht="15.75" customHeight="1">
       <c r="A233" s="2" t="s">
         <v>697</v>
       </c>
@@ -5840,8 +5851,8 @@
         <v>804.0</v>
       </c>
     </row>
-    <row r="234">
-      <c r="A234" s="2" t="s">
+    <row r="234" ht="15.75" customHeight="1">
+      <c r="A234" s="3" t="s">
         <v>700</v>
       </c>
       <c r="B234" s="2" t="s">
@@ -5854,8 +5865,8 @@
         <v>784.0</v>
       </c>
     </row>
-    <row r="235">
-      <c r="A235" s="2" t="s">
+    <row r="235" ht="15.75" customHeight="1">
+      <c r="A235" s="3" t="s">
         <v>703</v>
       </c>
       <c r="B235" s="2" t="s">
@@ -5868,8 +5879,8 @@
         <v>826.0</v>
       </c>
     </row>
-    <row r="236">
-      <c r="A236" s="2" t="s">
+    <row r="236" ht="15.75" customHeight="1">
+      <c r="A236" s="3" t="s">
         <v>706</v>
       </c>
       <c r="B236" s="2" t="s">
@@ -5882,8 +5893,8 @@
         <v>581.0</v>
       </c>
     </row>
-    <row r="237">
-      <c r="A237" s="2" t="s">
+    <row r="237" ht="15.75" customHeight="1">
+      <c r="A237" s="3" t="s">
         <v>709</v>
       </c>
       <c r="B237" s="2" t="s">
@@ -5896,7 +5907,7 @@
         <v>840.0</v>
       </c>
     </row>
-    <row r="238">
+    <row r="238" ht="15.75" customHeight="1">
       <c r="A238" s="2" t="s">
         <v>712</v>
       </c>
@@ -5910,7 +5921,7 @@
         <v>858.0</v>
       </c>
     </row>
-    <row r="239">
+    <row r="239" ht="15.75" customHeight="1">
       <c r="A239" s="2" t="s">
         <v>715</v>
       </c>
@@ -5924,7 +5935,7 @@
         <v>860.0</v>
       </c>
     </row>
-    <row r="240">
+    <row r="240" ht="15.75" customHeight="1">
       <c r="A240" s="2" t="s">
         <v>718</v>
       </c>
@@ -5938,8 +5949,8 @@
         <v>548.0</v>
       </c>
     </row>
-    <row r="241">
-      <c r="A241" s="2" t="s">
+    <row r="241" ht="15.75" customHeight="1">
+      <c r="A241" s="3" t="s">
         <v>721</v>
       </c>
       <c r="B241" s="2" t="s">
@@ -5952,7 +5963,7 @@
         <v>862.0</v>
       </c>
     </row>
-    <row r="242">
+    <row r="242" ht="15.75" customHeight="1">
       <c r="A242" s="2" t="s">
         <v>724</v>
       </c>
@@ -5966,7 +5977,7 @@
         <v>704.0</v>
       </c>
     </row>
-    <row r="243">
+    <row r="243" ht="15.75" customHeight="1">
       <c r="A243" s="2" t="s">
         <v>727</v>
       </c>
@@ -5980,7 +5991,7 @@
         <v>92.0</v>
       </c>
     </row>
-    <row r="244">
+    <row r="244" ht="15.75" customHeight="1">
       <c r="A244" s="2" t="s">
         <v>730</v>
       </c>
@@ -5994,7 +6005,7 @@
         <v>850.0</v>
       </c>
     </row>
-    <row r="245">
+    <row r="245" ht="15.75" customHeight="1">
       <c r="A245" s="2" t="s">
         <v>733</v>
       </c>
@@ -6008,7 +6019,7 @@
         <v>876.0</v>
       </c>
     </row>
-    <row r="246">
+    <row r="246" ht="15.75" customHeight="1">
       <c r="A246" s="2" t="s">
         <v>736</v>
       </c>
@@ -6022,7 +6033,7 @@
         <v>732.0</v>
       </c>
     </row>
-    <row r="247">
+    <row r="247" ht="15.75" customHeight="1">
       <c r="A247" s="2" t="s">
         <v>739</v>
       </c>
@@ -6036,7 +6047,7 @@
         <v>887.0</v>
       </c>
     </row>
-    <row r="248">
+    <row r="248" ht="15.75" customHeight="1">
       <c r="A248" s="2" t="s">
         <v>742</v>
       </c>
@@ -6050,7 +6061,7 @@
         <v>894.0</v>
       </c>
     </row>
-    <row r="249">
+    <row r="249" ht="15.75" customHeight="1">
       <c r="A249" s="2" t="s">
         <v>745</v>
       </c>
@@ -6064,7 +6075,7 @@
         <v>716.0</v>
       </c>
     </row>
-    <row r="250">
+    <row r="250" ht="15.75" customHeight="1">
       <c r="A250" s="2" t="s">
         <v>748</v>
       </c>
@@ -6078,11 +6089,760 @@
         <v>248.0</v>
       </c>
     </row>
-    <row r="257">
-      <c r="A257" s="3" t="s">
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1">
+      <c r="A257" s="4" t="s">
         <v>751</v>
       </c>
     </row>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>